<commit_message>
stacknew fields added in ui and in exel
</commit_message>
<xml_diff>
--- a/src/main/resources/static/newAssets/documents/Ambient.xlsx
+++ b/src/main/resources/static/newAssets/documents/Ambient.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\kyc\kyc\src\main\resources\static\newAssets\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF4F998-DAB8-4804-9E21-701E1F5C876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7188"/>
+    <workbookView xWindow="480" yWindow="840" windowWidth="20010" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ambient" sheetId="1" r:id="rId1"/>
@@ -47,8 +53,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,28 +858,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -892,14 +898,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1"/>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$4</xm:f>
           </x14:formula1>
@@ -912,31 +918,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>

</xml_diff>